<commit_message>
preprocess update, geo footprint page is done
</commit_message>
<xml_diff>
--- a/backend/datasets/agencies_preprocessed.xlsx
+++ b/backend/datasets/agencies_preprocessed.xlsx
@@ -480,7 +480,7 @@
         <v>1856</v>
       </c>
       <c r="B2" t="n">
-        <v>1921</v>
+        <v>1957</v>
       </c>
       <c r="C2" t="inlineStr">
         <is>
@@ -684,7 +684,7 @@
         <v>1862</v>
       </c>
       <c r="B8" t="n">
-        <v>1880</v>
+        <v>1954</v>
       </c>
       <c r="C8" t="inlineStr">
         <is>
@@ -851,12 +851,14 @@
     </row>
     <row r="13">
       <c r="A13" t="n">
-        <v>1865</v>
-      </c>
-      <c r="B13" t="inlineStr"/>
+        <v>1863</v>
+      </c>
+      <c r="B13" t="n">
+        <v>1974</v>
+      </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Isparta</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
@@ -866,31 +868,25 @@
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>Unknown, Isparta, Turkey</t>
-        </is>
-      </c>
-      <c r="G13" t="n">
-        <v>37.9465412</v>
-      </c>
-      <c r="H13" t="n">
-        <v>30.9602093</v>
-      </c>
+          <t>Unknown, Unknown, Unknown</t>
+        </is>
+      </c>
+      <c r="G13" t="inlineStr"/>
+      <c r="H13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="n">
-        <v>1867</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1958</v>
-      </c>
+        <v>1865</v>
+      </c>
+      <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>Alexandria</t>
+          <t>Isparta</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -900,31 +896,31 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>Unknown, Alexandria, Egypt</t>
+          <t>Unknown, Isparta, Turkey</t>
         </is>
       </c>
       <c r="G14" t="n">
-        <v>31.1991806</v>
+        <v>37.9465412</v>
       </c>
       <c r="H14" t="n">
-        <v>29.8951716</v>
+        <v>30.9602093</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
-        <v>1868</v>
+        <v>1867</v>
       </c>
       <c r="B15" t="n">
-        <v>1950</v>
+        <v>1958</v>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>Paris</t>
+          <t>Alexandria</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
@@ -934,31 +930,31 @@
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>Unknown, Paris, France</t>
+          <t>Unknown, Alexandria, Egypt</t>
         </is>
       </c>
       <c r="G15" t="n">
-        <v>48.8534951</v>
+        <v>31.1991806</v>
       </c>
       <c r="H15" t="n">
-        <v>2.3483915</v>
+        <v>29.8951716</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>1869</v>
+        <v>1868</v>
       </c>
       <c r="B16" t="n">
-        <v>1941</v>
+        <v>1950</v>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>Antalya</t>
+          <t>Paris</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
@@ -968,31 +964,31 @@
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Unknown, Antalya, Turkey</t>
+          <t>Unknown, Paris, France</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>36.8865728</v>
+        <v>48.8588897</v>
       </c>
       <c r="H16" t="n">
-        <v>30.7030242</v>
+        <v>2.320041</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
-        <v>1872</v>
+        <v>1869</v>
       </c>
       <c r="B17" t="n">
-        <v>1948</v>
+        <v>1941</v>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>Port Said</t>
+          <t>Antalya</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
@@ -1002,53 +998,53 @@
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>Unknown, Port Said, Egypt</t>
+          <t>Unknown, Antalya, Turkey</t>
         </is>
       </c>
       <c r="G17" t="n">
-        <v>31.263235</v>
+        <v>36.8865728</v>
       </c>
       <c r="H17" t="n">
-        <v>32.305505</v>
+        <v>30.7030242</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
-        <v>1874</v>
+        <v>1872</v>
       </c>
       <c r="B18" t="n">
-        <v>1967</v>
+        <v>1948</v>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>İstanbul</t>
+          <t>Port Said</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>Fatih</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>Fatih, İstanbul, Turkey</t>
+          <t>Unknown, Port Said, Egypt</t>
         </is>
       </c>
       <c r="G18" t="n">
-        <v>41.0192846</v>
+        <v>31.263235</v>
       </c>
       <c r="H18" t="n">
-        <v>28.9479296</v>
+        <v>32.305505</v>
       </c>
     </row>
     <row r="19">
@@ -1056,45 +1052,45 @@
         <v>1874</v>
       </c>
       <c r="B19" t="n">
-        <v>1957</v>
+        <v>1967</v>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>Jaffa</t>
+          <t>İstanbul</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Fatih</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>Unknown, Jaffa, Israel</t>
+          <t>Fatih, İstanbul, Turkey</t>
         </is>
       </c>
       <c r="G19" t="n">
-        <v>32.0443395</v>
+        <v>41.0192846</v>
       </c>
       <c r="H19" t="n">
-        <v>34.7509908</v>
+        <v>28.9479296</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="n">
-        <v>1875</v>
+        <v>1874</v>
       </c>
       <c r="B20" t="n">
-        <v>1954</v>
+        <v>1957</v>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>Bursa</t>
+          <t>Jaffa</t>
         </is>
       </c>
       <c r="D20" t="inlineStr">
@@ -1104,19 +1100,19 @@
       </c>
       <c r="E20" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>Unknown, Bursa, Turkey</t>
+          <t>Unknown, Jaffa, Israel</t>
         </is>
       </c>
       <c r="G20" t="n">
-        <v>39.9895878</v>
+        <v>32.0443395</v>
       </c>
       <c r="H20" t="n">
-        <v>28.8944669</v>
+        <v>34.7509908</v>
       </c>
     </row>
     <row r="21">
@@ -1124,11 +1120,11 @@
         <v>1875</v>
       </c>
       <c r="B21" t="n">
-        <v>1880</v>
+        <v>1954</v>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>Damascus</t>
+          <t>Bursa</t>
         </is>
       </c>
       <c r="D21" t="inlineStr">
@@ -1138,19 +1134,19 @@
       </c>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>Unknown, Damascus, Syria</t>
+          <t>Unknown, Bursa, Turkey</t>
         </is>
       </c>
       <c r="G21" t="n">
-        <v>33.5130695</v>
+        <v>39.9895878</v>
       </c>
       <c r="H21" t="n">
-        <v>36.3095814</v>
+        <v>28.8944669</v>
       </c>
     </row>
     <row r="22">
@@ -1158,11 +1154,11 @@
         <v>1875</v>
       </c>
       <c r="B22" t="n">
-        <v>1956</v>
+        <v>1942</v>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Edirne</t>
+          <t>Damascus</t>
         </is>
       </c>
       <c r="D22" t="inlineStr">
@@ -1172,19 +1168,19 @@
       </c>
       <c r="E22" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Syria</t>
         </is>
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>Unknown, Edirne, Turkey</t>
+          <t>Unknown, Damascus, Syria</t>
         </is>
       </c>
       <c r="G22" t="n">
-        <v>41.6759327</v>
+        <v>33.5130695</v>
       </c>
       <c r="H22" t="n">
-        <v>26.5587225</v>
+        <v>36.3095814</v>
       </c>
     </row>
     <row r="23">
@@ -1192,11 +1188,11 @@
         <v>1875</v>
       </c>
       <c r="B23" t="n">
-        <v>1880</v>
+        <v>1956</v>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>Ruse</t>
+          <t>Edirne</t>
         </is>
       </c>
       <c r="D23" t="inlineStr">
@@ -1206,31 +1202,31 @@
       </c>
       <c r="E23" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>Unknown, Ruse, Bulgaria</t>
+          <t>Unknown, Edirne, Turkey</t>
         </is>
       </c>
       <c r="G23" t="n">
-        <v>43.8480413</v>
+        <v>41.6759327</v>
       </c>
       <c r="H23" t="n">
-        <v>25.9542057</v>
+        <v>26.5587225</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="n">
-        <v>1878</v>
+        <v>1875</v>
       </c>
       <c r="B24" t="n">
-        <v>1899</v>
+        <v>1880</v>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>Plovdiv</t>
+          <t>Ruse</t>
         </is>
       </c>
       <c r="D24" t="inlineStr">
@@ -1245,60 +1241,60 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>Unknown, Plovdiv, Bulgaria</t>
+          <t>Unknown, Ruse, Bulgaria</t>
         </is>
       </c>
       <c r="G24" t="n">
-        <v>42.1418541</v>
+        <v>43.8480413</v>
       </c>
       <c r="H24" t="n">
-        <v>24.7499297</v>
+        <v>25.9542057</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="n">
-        <v>1879</v>
+        <v>1876</v>
       </c>
       <c r="B25" t="n">
-        <v>1936</v>
+        <v>1974</v>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>Limassol</t>
+          <t>İstanbul</t>
         </is>
       </c>
       <c r="D25" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Pera</t>
         </is>
       </c>
       <c r="E25" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>Unknown, Limassol, Cyprus</t>
+          <t>Pera, İstanbul, Turkey</t>
         </is>
       </c>
       <c r="G25" t="n">
-        <v>34.6852901</v>
+        <v>41.0284233</v>
       </c>
       <c r="H25" t="n">
-        <v>33.0332657</v>
+        <v>28.9736808</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="n">
-        <v>1879</v>
+        <v>1878</v>
       </c>
       <c r="B26" t="n">
-        <v>1967</v>
+        <v>1899</v>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>Nicosia</t>
+          <t>Plovdiv</t>
         </is>
       </c>
       <c r="D26" t="inlineStr">
@@ -1308,31 +1304,31 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>Unknown, Nicosia, Cyprus</t>
+          <t>Unknown, Plovdiv, Bulgaria</t>
         </is>
       </c>
       <c r="G26" t="n">
-        <v>35.1746503</v>
+        <v>42.1418541</v>
       </c>
       <c r="H26" t="n">
-        <v>33.3638783</v>
+        <v>24.7499297</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="n">
-        <v>1880</v>
+        <v>1879</v>
       </c>
       <c r="B27" t="n">
-        <v>1882</v>
+        <v>1936</v>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>Varna</t>
+          <t>Limassol</t>
         </is>
       </c>
       <c r="D27" t="inlineStr">
@@ -1342,138 +1338,138 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>Unknown, Varna, Bulgaria</t>
+          <t>Unknown, Limassol, Cyprus</t>
         </is>
       </c>
       <c r="G27" t="n">
-        <v>43.2073873</v>
+        <v>34.6852901</v>
       </c>
       <c r="H27" t="n">
-        <v>27.9166653</v>
+        <v>33.0332657</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>1881</v>
+        <v>1879</v>
       </c>
       <c r="B28" t="n">
-        <v>1898</v>
+        <v>1967</v>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>Aydın</t>
+          <t>Nicosia</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Nazilli</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>Nazilli, Aydın, Turkey</t>
+          <t>Unknown, Nicosia, Cyprus</t>
         </is>
       </c>
       <c r="G28" t="n">
-        <v>37.9097512</v>
+        <v>35.1746503</v>
       </c>
       <c r="H28" t="n">
-        <v>28.3242062</v>
+        <v>33.3638783</v>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>1886</v>
+        <v>1880</v>
       </c>
       <c r="B29" t="n">
-        <v>1953</v>
+        <v>1882</v>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>İstanbul</t>
+          <t>Varna</t>
         </is>
       </c>
       <c r="D29" t="inlineStr">
         <is>
-          <t>Yeni Cami</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E29" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>Yeni Cami, İstanbul, Turkey</t>
+          <t>Unknown, Varna, Bulgaria</t>
         </is>
       </c>
       <c r="G29" t="n">
-        <v>41.0841248</v>
+        <v>43.2073873</v>
       </c>
       <c r="H29" t="n">
-        <v>29.0789477</v>
+        <v>27.9166653</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="n">
-        <v>1887</v>
+        <v>1881</v>
       </c>
       <c r="B30" t="n">
-        <v>1958</v>
+        <v>1947</v>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>Cairo</t>
+          <t>Aydın</t>
         </is>
       </c>
       <c r="D30" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Nazilli</t>
         </is>
       </c>
       <c r="E30" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>Unknown, Cairo, Egypt</t>
+          <t>Nazilli, Aydın, Turkey</t>
         </is>
       </c>
       <c r="G30" t="n">
-        <v>30.0443879</v>
+        <v>37.9097512</v>
       </c>
       <c r="H30" t="n">
-        <v>31.2357257</v>
+        <v>28.3242062</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="n">
-        <v>1889</v>
+        <v>1881</v>
       </c>
       <c r="B31" t="n">
-        <v>1950</v>
+        <v>1957</v>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>Adana</t>
+          <t>Kastamonu</t>
         </is>
       </c>
       <c r="D31" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>İnebolu</t>
         </is>
       </c>
       <c r="E31" t="inlineStr">
@@ -1483,31 +1479,31 @@
       </c>
       <c r="F31" t="inlineStr">
         <is>
-          <t>Unknown, Adana, Turkey</t>
+          <t>İnebolu, Kastamonu, Turkey</t>
         </is>
       </c>
       <c r="G31" t="n">
-        <v>36.9863599</v>
+        <v>41.9785763</v>
       </c>
       <c r="H31" t="n">
-        <v>35.3252861</v>
+        <v>33.7599031</v>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>1889</v>
+        <v>1886</v>
       </c>
       <c r="B32" t="n">
-        <v>1951</v>
+        <v>1953</v>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Konya</t>
+          <t>İstanbul</t>
         </is>
       </c>
       <c r="D32" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Yeni Cami</t>
         </is>
       </c>
       <c r="E32" t="inlineStr">
@@ -1517,26 +1513,26 @@
       </c>
       <c r="F32" t="inlineStr">
         <is>
-          <t>Unknown, Konya, Turkey</t>
+          <t>Yeni Cami, İstanbul, Turkey</t>
         </is>
       </c>
       <c r="G32" t="n">
-        <v>37.872734</v>
+        <v>41.0841248</v>
       </c>
       <c r="H32" t="n">
-        <v>32.4924376</v>
+        <v>29.0789477</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="n">
-        <v>1890</v>
+        <v>1887</v>
       </c>
       <c r="B33" t="n">
-        <v>1950</v>
+        <v>1958</v>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>Denizli</t>
+          <t>Cairo</t>
         </is>
       </c>
       <c r="D33" t="inlineStr">
@@ -1546,29 +1542,31 @@
       </c>
       <c r="E33" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="F33" t="inlineStr">
         <is>
-          <t>Unknown, Denizli, Turkey</t>
+          <t>Unknown, Cairo, Egypt</t>
         </is>
       </c>
       <c r="G33" t="n">
-        <v>37.8275892</v>
+        <v>30.0443879</v>
       </c>
       <c r="H33" t="n">
-        <v>29.2389539</v>
+        <v>31.2357257</v>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="n">
-        <v>1890</v>
-      </c>
-      <c r="B34" t="inlineStr"/>
+        <v>1888</v>
+      </c>
+      <c r="B34" t="n">
+        <v>1950</v>
+      </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>Muğla</t>
+          <t>Adana</t>
         </is>
       </c>
       <c r="D34" t="inlineStr">
@@ -1583,26 +1581,26 @@
       </c>
       <c r="F34" t="inlineStr">
         <is>
-          <t>Unknown, Muğla, Turkey</t>
+          <t>Unknown, Adana, Turkey</t>
         </is>
       </c>
       <c r="G34" t="n">
-        <v>37.1642053</v>
+        <v>36.9863599</v>
       </c>
       <c r="H34" t="n">
-        <v>28.2624288</v>
+        <v>35.3252861</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="n">
-        <v>1890</v>
+        <v>1889</v>
       </c>
       <c r="B35" t="n">
-        <v>1899</v>
+        <v>1951</v>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>Sofia</t>
+          <t>Konya</t>
         </is>
       </c>
       <c r="D35" t="inlineStr">
@@ -1612,36 +1610,36 @@
       </c>
       <c r="E35" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F35" t="inlineStr">
         <is>
-          <t>Unknown, Sofia, Bulgaria</t>
+          <t>Unknown, Konya, Turkey</t>
         </is>
       </c>
       <c r="G35" t="n">
-        <v>42.6977028</v>
+        <v>37.872734</v>
       </c>
       <c r="H35" t="n">
-        <v>23.3217359</v>
+        <v>32.4924376</v>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="n">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="B36" t="n">
-        <v>1974</v>
+        <v>1950</v>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>İstanbul</t>
+          <t>Denizli</t>
         </is>
       </c>
       <c r="D36" t="inlineStr">
         <is>
-          <t>Pera</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E36" t="inlineStr">
@@ -1651,26 +1649,24 @@
       </c>
       <c r="F36" t="inlineStr">
         <is>
-          <t>Pera, İstanbul, Turkey</t>
+          <t>Unknown, Denizli, Turkey</t>
         </is>
       </c>
       <c r="G36" t="n">
-        <v>41.0284233</v>
+        <v>37.8275892</v>
       </c>
       <c r="H36" t="n">
-        <v>28.9736808</v>
+        <v>29.2389539</v>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="n">
-        <v>1891</v>
-      </c>
-      <c r="B37" t="n">
-        <v>1938</v>
-      </c>
+        <v>1890</v>
+      </c>
+      <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Balıkesir</t>
+          <t>Muğla</t>
         </is>
       </c>
       <c r="D37" t="inlineStr">
@@ -1685,26 +1681,26 @@
       </c>
       <c r="F37" t="inlineStr">
         <is>
-          <t>Unknown, Balıkesir, Turkey</t>
+          <t>Unknown, Muğla, Turkey</t>
         </is>
       </c>
       <c r="G37" t="n">
-        <v>39.5400798</v>
+        <v>37.1642053</v>
       </c>
       <c r="H37" t="n">
-        <v>28.0228793</v>
+        <v>28.2624288</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="n">
-        <v>1891</v>
+        <v>1890</v>
       </c>
       <c r="B38" t="n">
-        <v>1956</v>
+        <v>1953</v>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>Samsun</t>
+          <t>Sofia</t>
         </is>
       </c>
       <c r="D38" t="inlineStr">
@@ -1714,19 +1710,19 @@
       </c>
       <c r="E38" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="F38" t="inlineStr">
         <is>
-          <t>Unknown, Samsun, Turkey</t>
+          <t>Unknown, Sofia, Bulgaria</t>
         </is>
       </c>
       <c r="G38" t="n">
-        <v>41.2303557</v>
+        <v>42.6977028</v>
       </c>
       <c r="H38" t="n">
-        <v>35.9683338</v>
+        <v>23.3217359</v>
       </c>
     </row>
     <row r="39">
@@ -1734,11 +1730,11 @@
         <v>1891</v>
       </c>
       <c r="B39" t="n">
-        <v>1958</v>
+        <v>1938</v>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>Trabzon</t>
+          <t>Balıkesir</t>
         </is>
       </c>
       <c r="D39" t="inlineStr">
@@ -1753,14 +1749,14 @@
       </c>
       <c r="F39" t="inlineStr">
         <is>
-          <t>Unknown, Trabzon, Turkey</t>
+          <t>Unknown, Balıkesir, Turkey</t>
         </is>
       </c>
       <c r="G39" t="n">
-        <v>41.0054605</v>
+        <v>39.5400798</v>
       </c>
       <c r="H39" t="n">
-        <v>39.7301463</v>
+        <v>28.0228793</v>
       </c>
     </row>
     <row r="40">
@@ -1768,11 +1764,11 @@
         <v>1891</v>
       </c>
       <c r="B40" t="n">
-        <v>1932</v>
+        <v>1958</v>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Uşak</t>
+          <t>Kütahya</t>
         </is>
       </c>
       <c r="D40" t="inlineStr">
@@ -1787,26 +1783,26 @@
       </c>
       <c r="F40" t="inlineStr">
         <is>
-          <t>Unknown, Uşak, Turkey</t>
+          <t>Unknown, Kütahya, Turkey</t>
         </is>
       </c>
       <c r="G40" t="n">
-        <v>38.5768902</v>
+        <v>39.2522508</v>
       </c>
       <c r="H40" t="n">
-        <v>29.3729779</v>
+        <v>29.4937732</v>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="n">
-        <v>1892</v>
+        <v>1891</v>
       </c>
       <c r="B41" t="n">
-        <v>1899</v>
+        <v>1956</v>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>Ruse</t>
+          <t>Samsun</t>
         </is>
       </c>
       <c r="D41" t="inlineStr">
@@ -1816,31 +1812,31 @@
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>Bulgaria</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F41" t="inlineStr">
         <is>
-          <t>Unknown, Ruse, Bulgaria</t>
+          <t>Unknown, Samsun, Turkey</t>
         </is>
       </c>
       <c r="G41" t="n">
-        <v>43.8480413</v>
+        <v>41.2303557</v>
       </c>
       <c r="H41" t="n">
-        <v>25.9542057</v>
+        <v>35.9683338</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="n">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="B42" t="n">
-        <v>1956</v>
+        <v>1958</v>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>Baghdad</t>
+          <t>Trabzon</t>
         </is>
       </c>
       <c r="D42" t="inlineStr">
@@ -1850,31 +1846,31 @@
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>Iraq</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F42" t="inlineStr">
         <is>
-          <t>Unknown, Baghdad, Iraq</t>
+          <t>Unknown, Trabzon, Turkey</t>
         </is>
       </c>
       <c r="G42" t="n">
-        <v>33.3061701</v>
+        <v>41.0054605</v>
       </c>
       <c r="H42" t="n">
-        <v>44.3872213</v>
+        <v>39.7301463</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="n">
-        <v>1893</v>
+        <v>1891</v>
       </c>
       <c r="B43" t="n">
-        <v>1957</v>
+        <v>1932</v>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Uşak</t>
         </is>
       </c>
       <c r="D43" t="inlineStr">
@@ -1884,31 +1880,31 @@
       </c>
       <c r="E43" t="inlineStr">
         <is>
-          <t>Iraq</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F43" t="inlineStr">
         <is>
-          <t>Unknown, Basra, Iraq</t>
+          <t>Unknown, Uşak, Turkey</t>
         </is>
       </c>
       <c r="G43" t="n">
-        <v>30.4952371</v>
+        <v>38.5768902</v>
       </c>
       <c r="H43" t="n">
-        <v>47.8090981</v>
+        <v>29.3729779</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="n">
-        <v>1894</v>
+        <v>1892</v>
       </c>
       <c r="B44" t="n">
-        <v>1943</v>
+        <v>1932</v>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>Aleppo</t>
+          <t>Bilecik</t>
         </is>
       </c>
       <c r="D44" t="inlineStr">
@@ -1918,31 +1914,31 @@
       </c>
       <c r="E44" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F44" t="inlineStr">
         <is>
-          <t>Unknown, Aleppo, Syria</t>
+          <t>Unknown, Bilecik, Turkey</t>
         </is>
       </c>
       <c r="G44" t="n">
-        <v>36.19924</v>
+        <v>40.1543234</v>
       </c>
       <c r="H44" t="n">
-        <v>37.1637253</v>
+        <v>30.1479907</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="n">
-        <v>1894</v>
+        <v>1892</v>
       </c>
       <c r="B45" t="n">
-        <v>1965</v>
+        <v>1899</v>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>Mersin</t>
+          <t>Ruse</t>
         </is>
       </c>
       <c r="D45" t="inlineStr">
@@ -1952,31 +1948,31 @@
       </c>
       <c r="E45" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Bulgaria</t>
         </is>
       </c>
       <c r="F45" t="inlineStr">
         <is>
-          <t>Unknown, Mersin, Turkey</t>
+          <t>Unknown, Ruse, Bulgaria</t>
         </is>
       </c>
       <c r="G45" t="n">
-        <v>36.7978381</v>
+        <v>43.8480413</v>
       </c>
       <c r="H45" t="n">
-        <v>34.6298391</v>
+        <v>25.9542057</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="n">
-        <v>1895</v>
+        <v>1892</v>
       </c>
       <c r="B46" t="n">
-        <v>1958</v>
+        <v>1934</v>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>Ankara</t>
+          <t>Şanlıurfa</t>
         </is>
       </c>
       <c r="D46" t="inlineStr">
@@ -1991,60 +1987,60 @@
       </c>
       <c r="F46" t="inlineStr">
         <is>
-          <t>Unknown, Ankara, Turkey</t>
+          <t>Unknown, Şanlıurfa, Turkey</t>
         </is>
       </c>
       <c r="G46" t="n">
-        <v>39.9207759</v>
+        <v>37.2595198</v>
       </c>
       <c r="H46" t="n">
-        <v>32.8540497</v>
+        <v>39.0408174</v>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="n">
-        <v>1898</v>
+        <v>1893</v>
       </c>
       <c r="B47" t="n">
-        <v>1921</v>
+        <v>1926</v>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>Lesbos</t>
+          <t>Afyonkarahisar</t>
         </is>
       </c>
       <c r="D47" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Bolvadin</t>
         </is>
       </c>
       <c r="E47" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F47" t="inlineStr">
         <is>
-          <t>Unknown, Lesbos, Greece</t>
+          <t>Bolvadin, Afyonkarahisar, Turkey</t>
         </is>
       </c>
       <c r="G47" t="n">
-        <v>39.1758418</v>
+        <v>38.7115866</v>
       </c>
       <c r="H47" t="n">
-        <v>25.9989135</v>
+        <v>31.0454865</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="n">
-        <v>1898</v>
+        <v>1893</v>
       </c>
       <c r="B48" t="n">
-        <v>1939</v>
+        <v>1956</v>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>Mytilene</t>
+          <t>Baghdad</t>
         </is>
       </c>
       <c r="D48" t="inlineStr">
@@ -2054,31 +2050,31 @@
       </c>
       <c r="E48" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Iraq</t>
         </is>
       </c>
       <c r="F48" t="inlineStr">
         <is>
-          <t>Unknown, Mytilene, Greece</t>
+          <t>Unknown, Baghdad, Iraq</t>
         </is>
       </c>
       <c r="G48" t="n">
-        <v>39.1037355</v>
+        <v>33.3061701</v>
       </c>
       <c r="H48" t="n">
-        <v>26.554788</v>
+        <v>44.3872213</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="n">
-        <v>1899</v>
+        <v>1893</v>
       </c>
       <c r="B49" t="n">
-        <v>1933</v>
+        <v>1957</v>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>Kastamonu</t>
+          <t>Basra</t>
         </is>
       </c>
       <c r="D49" t="inlineStr">
@@ -2088,31 +2084,31 @@
       </c>
       <c r="E49" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Iraq</t>
         </is>
       </c>
       <c r="F49" t="inlineStr">
         <is>
-          <t>Unknown, Kastamonu, Turkey</t>
+          <t>Unknown, Basra, Iraq</t>
         </is>
       </c>
       <c r="G49" t="n">
-        <v>41.3680217</v>
+        <v>30.4952371</v>
       </c>
       <c r="H49" t="n">
-        <v>33.7619177</v>
+        <v>47.8090981</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="n">
-        <v>1899</v>
+        <v>1894</v>
       </c>
       <c r="B50" t="n">
-        <v>1933</v>
+        <v>1943</v>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>Sivas</t>
+          <t>Aleppo</t>
         </is>
       </c>
       <c r="D50" t="inlineStr">
@@ -2122,31 +2118,31 @@
       </c>
       <c r="E50" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Syria</t>
         </is>
       </c>
       <c r="F50" t="inlineStr">
         <is>
-          <t>Unknown, Sivas, Turkey</t>
+          <t>Unknown, Aleppo, Syria</t>
         </is>
       </c>
       <c r="G50" t="n">
-        <v>39.4191717</v>
+        <v>36.19924</v>
       </c>
       <c r="H50" t="n">
-        <v>37.1012388</v>
+        <v>37.1637253</v>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="n">
-        <v>1900</v>
+        <v>1894</v>
       </c>
       <c r="B51" t="n">
-        <v>1952</v>
+        <v>1965</v>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Mersin</t>
         </is>
       </c>
       <c r="D51" t="inlineStr">
@@ -2156,31 +2152,31 @@
       </c>
       <c r="E51" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F51" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, Greece</t>
+          <t>Unknown, Mersin, Turkey</t>
         </is>
       </c>
       <c r="G51" t="n">
-        <v>38.9953683</v>
+        <v>36.7978381</v>
       </c>
       <c r="H51" t="n">
-        <v>21.9877132</v>
+        <v>34.6298391</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>1903</v>
+        <v>1895</v>
       </c>
       <c r="B52" t="n">
-        <v>1914</v>
+        <v>1958</v>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>Bitola</t>
+          <t>Ankara</t>
         </is>
       </c>
       <c r="D52" t="inlineStr">
@@ -2190,31 +2186,31 @@
       </c>
       <c r="E52" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F52" t="inlineStr">
         <is>
-          <t>Unknown, Bitola, North Macedonia</t>
+          <t>Unknown, Ankara, Turkey</t>
         </is>
       </c>
       <c r="G52" t="n">
-        <v>41.0316005</v>
+        <v>39.9207759</v>
       </c>
       <c r="H52" t="n">
-        <v>21.3302511</v>
+        <v>32.8540497</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="n">
-        <v>1903</v>
+        <v>1898</v>
       </c>
       <c r="B53" t="n">
-        <v>1958</v>
+        <v>1921</v>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Lesbos</t>
         </is>
       </c>
       <c r="D53" t="inlineStr">
@@ -2224,31 +2220,31 @@
       </c>
       <c r="E53" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F53" t="inlineStr">
         <is>
-          <t>Unknown, Haifa, Israel</t>
+          <t>Unknown, Lesbos, Greece</t>
         </is>
       </c>
       <c r="G53" t="n">
-        <v>32.8191218</v>
+        <v>39.1758418</v>
       </c>
       <c r="H53" t="n">
-        <v>34.9983856</v>
+        <v>25.9989135</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="n">
-        <v>1903</v>
+        <v>1898</v>
       </c>
       <c r="B54" t="n">
-        <v>1914</v>
+        <v>1939</v>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>Skopje</t>
+          <t>Mytilene</t>
         </is>
       </c>
       <c r="D54" t="inlineStr">
@@ -2258,36 +2254,36 @@
       </c>
       <c r="E54" t="inlineStr">
         <is>
-          <t>North Macedonia</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F54" t="inlineStr">
         <is>
-          <t>Unknown, Skopje, North Macedonia</t>
+          <t>Unknown, Mytilene, Greece</t>
         </is>
       </c>
       <c r="G54" t="n">
-        <v>41.9961816</v>
+        <v>39.1037355</v>
       </c>
       <c r="H54" t="n">
-        <v>21.4319213</v>
+        <v>26.554788</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="n">
-        <v>1904</v>
+        <v>1899</v>
       </c>
       <c r="B55" t="n">
-        <v>1957</v>
+        <v>1954</v>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>Konya</t>
+          <t>Gaziantep</t>
         </is>
       </c>
       <c r="D55" t="inlineStr">
         <is>
-          <t>Akşehir</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E55" t="inlineStr">
@@ -2297,26 +2293,26 @@
       </c>
       <c r="F55" t="inlineStr">
         <is>
-          <t>Akşehir, Konya, Turkey</t>
+          <t>Unknown, Gaziantep, Turkey</t>
         </is>
       </c>
       <c r="G55" t="n">
-        <v>38.3588503</v>
+        <v>37.0628317</v>
       </c>
       <c r="H55" t="n">
-        <v>31.4201959</v>
+        <v>37.3792617</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="n">
-        <v>1904</v>
+        <v>1899</v>
       </c>
       <c r="B56" t="n">
-        <v>1914</v>
+        <v>1933</v>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>Alexandroupoli</t>
+          <t>Kastamonu</t>
         </is>
       </c>
       <c r="D56" t="inlineStr">
@@ -2326,31 +2322,31 @@
       </c>
       <c r="E56" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F56" t="inlineStr">
         <is>
-          <t>Unknown, Alexandroupoli, Greece</t>
+          <t>Unknown, Kastamonu, Turkey</t>
         </is>
       </c>
       <c r="G56" t="n">
-        <v>40.845666</v>
+        <v>41.3680217</v>
       </c>
       <c r="H56" t="n">
-        <v>25.8778814</v>
+        <v>33.7619177</v>
       </c>
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>1904</v>
+        <v>1899</v>
       </c>
       <c r="B57" t="n">
-        <v>1955</v>
+        <v>1957</v>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Eskişehir</t>
+          <t>Ordu</t>
         </is>
       </c>
       <c r="D57" t="inlineStr">
@@ -2365,24 +2361,26 @@
       </c>
       <c r="F57" t="inlineStr">
         <is>
-          <t>Unknown, Eskişehir, Turkey</t>
+          <t>Unknown, Ordu, Turkey</t>
         </is>
       </c>
       <c r="G57" t="n">
-        <v>39.7743941</v>
+        <v>40.8292569</v>
       </c>
       <c r="H57" t="n">
-        <v>30.519116</v>
+        <v>37.4082764</v>
       </c>
     </row>
     <row r="58">
       <c r="A58" t="n">
-        <v>1904</v>
-      </c>
-      <c r="B58" t="inlineStr"/>
+        <v>1899</v>
+      </c>
+      <c r="B58" t="n">
+        <v>1933</v>
+      </c>
       <c r="C58" t="inlineStr">
         <is>
-          <t>Jerusalem</t>
+          <t>Sivas</t>
         </is>
       </c>
       <c r="D58" t="inlineStr">
@@ -2392,31 +2390,31 @@
       </c>
       <c r="E58" t="inlineStr">
         <is>
-          <t>Palestine</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F58" t="inlineStr">
         <is>
-          <t>Unknown, Jerusalem, Palestine</t>
+          <t>Unknown, Sivas, Turkey</t>
         </is>
       </c>
       <c r="G58" t="n">
-        <v>33.6132575</v>
+        <v>39.4191717</v>
       </c>
       <c r="H58" t="n">
-        <v>-87.8553466</v>
+        <v>37.1012388</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="n">
-        <v>1904</v>
+        <v>1899</v>
       </c>
       <c r="B59" t="n">
-        <v>1932</v>
+        <v>1957</v>
       </c>
       <c r="C59" t="inlineStr">
         <is>
-          <t>Kavala</t>
+          <t>Skopje</t>
         </is>
       </c>
       <c r="D59" t="inlineStr">
@@ -2426,31 +2424,31 @@
       </c>
       <c r="E59" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="F59" t="inlineStr">
         <is>
-          <t>Unknown, Kavala, Greece</t>
+          <t>Unknown, Skopje, North Macedonia</t>
         </is>
       </c>
       <c r="G59" t="n">
-        <v>40.9369224</v>
+        <v>41.9961816</v>
       </c>
       <c r="H59" t="n">
-        <v>24.4122766</v>
+        <v>21.4319213</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="n">
-        <v>1904</v>
+        <v>1900</v>
       </c>
       <c r="B60" t="n">
-        <v>1921</v>
+        <v>1932</v>
       </c>
       <c r="C60" t="inlineStr">
         <is>
-          <t>Tripoli</t>
+          <t>Bitola</t>
         </is>
       </c>
       <c r="D60" t="inlineStr">
@@ -2460,31 +2458,31 @@
       </c>
       <c r="E60" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>North Macedonia</t>
         </is>
       </c>
       <c r="F60" t="inlineStr">
         <is>
-          <t>Unknown, Tripoli, Lebanon</t>
+          <t>Unknown, Bitola, North Macedonia</t>
         </is>
       </c>
       <c r="G60" t="n">
-        <v>34.4373616</v>
+        <v>41.0316005</v>
       </c>
       <c r="H60" t="n">
-        <v>35.8348551</v>
+        <v>21.3302511</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="n">
-        <v>1904</v>
+        <v>1900</v>
       </c>
       <c r="B61" t="n">
-        <v>1933</v>
+        <v>1928</v>
       </c>
       <c r="C61" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Jeddah</t>
         </is>
       </c>
       <c r="D61" t="inlineStr">
@@ -2494,70 +2492,70 @@
       </c>
       <c r="E61" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Saudi Arabia</t>
         </is>
       </c>
       <c r="F61" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, France</t>
+          <t>Unknown, Jeddah, Saudi Arabia</t>
         </is>
       </c>
       <c r="G61" t="n">
-        <v>46.603354</v>
+        <v>21.5504432</v>
       </c>
       <c r="H61" t="n">
-        <v>1.8883335</v>
+        <v>39.1742363</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="n">
-        <v>1905</v>
+        <v>1900</v>
       </c>
       <c r="B62" t="n">
-        <v>1955</v>
+        <v>1952</v>
       </c>
       <c r="C62" t="inlineStr">
         <is>
-          <t>Balıkesir</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D62" t="inlineStr">
         <is>
-          <t>Bandırma</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E62" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F62" t="inlineStr">
         <is>
-          <t>Bandırma, Balıkesir, Turkey</t>
+          <t>Unknown, Unknown, Greece</t>
         </is>
       </c>
       <c r="G62" t="n">
-        <v>40.3554705</v>
+        <v>38.9953683</v>
       </c>
       <c r="H62" t="n">
-        <v>27.9697603</v>
+        <v>21.9877132</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="n">
-        <v>1905</v>
+        <v>1901</v>
       </c>
       <c r="B63" t="n">
-        <v>1947</v>
+        <v>1955</v>
       </c>
       <c r="C63" t="inlineStr">
         <is>
-          <t>Aydın</t>
+          <t>Balıkesir</t>
         </is>
       </c>
       <c r="D63" t="inlineStr">
         <is>
-          <t>Nazilli</t>
+          <t>Bandırma</t>
         </is>
       </c>
       <c r="E63" t="inlineStr">
@@ -2567,26 +2565,26 @@
       </c>
       <c r="F63" t="inlineStr">
         <is>
-          <t>Nazilli, Aydın, Turkey</t>
+          <t>Bandırma, Balıkesir, Turkey</t>
         </is>
       </c>
       <c r="G63" t="n">
-        <v>37.9097512</v>
+        <v>40.3554705</v>
       </c>
       <c r="H63" t="n">
-        <v>28.3242062</v>
+        <v>27.9697603</v>
       </c>
     </row>
     <row r="64">
       <c r="A64" t="n">
-        <v>1905</v>
+        <v>1901</v>
       </c>
       <c r="B64" t="n">
-        <v>1932</v>
+        <v>1935</v>
       </c>
       <c r="C64" t="inlineStr">
         <is>
-          <t>Bilecik</t>
+          <t>Diyarbakır</t>
         </is>
       </c>
       <c r="D64" t="inlineStr">
@@ -2601,24 +2599,26 @@
       </c>
       <c r="F64" t="inlineStr">
         <is>
-          <t>Unknown, Bilecik, Turkey</t>
+          <t>Unknown, Diyarbakır, Turkey</t>
         </is>
       </c>
       <c r="G64" t="n">
-        <v>40.1543234</v>
+        <v>37.9162222</v>
       </c>
       <c r="H64" t="n">
-        <v>30.1479907</v>
+        <v>40.2363542</v>
       </c>
     </row>
     <row r="65">
       <c r="A65" t="n">
-        <v>1905</v>
-      </c>
-      <c r="B65" t="inlineStr"/>
+        <v>1901</v>
+      </c>
+      <c r="B65" t="n">
+        <v>1950</v>
+      </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Jaffa</t>
+          <t>Mosul</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
@@ -2628,70 +2628,70 @@
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>Palestine</t>
+          <t>Iraq</t>
         </is>
       </c>
       <c r="F65" t="inlineStr">
         <is>
-          <t>Unknown, Jaffa, Palestine</t>
+          <t>Unknown, Mosul, Iraq</t>
         </is>
       </c>
       <c r="G65" t="n">
-        <v>32.0539873</v>
+        <v>36.343694</v>
       </c>
       <c r="H65" t="n">
-        <v>34.75508</v>
+        <v>43.0997156</v>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>1905</v>
+        <v>1903</v>
       </c>
       <c r="B66" t="n">
-        <v>1958</v>
+        <v>1957</v>
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Jerusalem</t>
+          <t>Konya</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Akşehir</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>Israel</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F66" t="inlineStr">
         <is>
-          <t>Unknown, Jerusalem, Israel</t>
+          <t>Akşehir, Konya, Turkey</t>
         </is>
       </c>
       <c r="G66" t="n">
-        <v>31.7788472</v>
+        <v>38.3588503</v>
       </c>
       <c r="H66" t="n">
-        <v>35.2257856</v>
+        <v>31.4201959</v>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="n">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="B67" t="n">
-        <v>1907</v>
+        <v>1955</v>
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Mersin</t>
+          <t>Eskişehir</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Silifke</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
@@ -2701,26 +2701,26 @@
       </c>
       <c r="F67" t="inlineStr">
         <is>
-          <t>Silifke, Mersin, Turkey</t>
+          <t>Unknown, Eskişehir, Turkey</t>
         </is>
       </c>
       <c r="G67" t="n">
-        <v>36.3778166</v>
+        <v>39.7743941</v>
       </c>
       <c r="H67" t="n">
-        <v>33.9260372</v>
+        <v>30.519116</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="n">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="B68" t="n">
-        <v>1955</v>
+        <v>1958</v>
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>Erzurum</t>
+          <t>Haifa</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
@@ -2730,31 +2730,31 @@
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="F68" t="inlineStr">
         <is>
-          <t>Unknown, Erzurum, Turkey</t>
+          <t>Unknown, Haifa, Israel</t>
         </is>
       </c>
       <c r="G68" t="n">
-        <v>39.90632</v>
+        <v>32.8191218</v>
       </c>
       <c r="H68" t="n">
-        <v>41.2727715</v>
+        <v>34.9983856</v>
       </c>
     </row>
     <row r="69">
       <c r="A69" t="n">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="B69" t="n">
-        <v>1947</v>
+        <v>1950</v>
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Famagusta</t>
+          <t>Hama</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
@@ -2764,31 +2764,31 @@
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Syria</t>
         </is>
       </c>
       <c r="F69" t="inlineStr">
         <is>
-          <t>Unknown, Famagusta, Cyprus</t>
+          <t>Unknown, Hama, Syria</t>
         </is>
       </c>
       <c r="G69" t="n">
-        <v>35.1205261</v>
+        <v>35.1343368</v>
       </c>
       <c r="H69" t="n">
-        <v>33.9387919</v>
+        <v>36.7496276</v>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="n">
-        <v>1906</v>
+        <v>1903</v>
       </c>
       <c r="B70" t="n">
-        <v>1954</v>
+        <v>1957</v>
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Gaziantep</t>
+          <t>Tekirdağ</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
@@ -2803,31 +2803,31 @@
       </c>
       <c r="F70" t="inlineStr">
         <is>
-          <t>Unknown, Gaziantep, Turkey</t>
+          <t>Unknown, Tekirdağ, Turkey</t>
         </is>
       </c>
       <c r="G70" t="n">
-        <v>37.0628317</v>
+        <v>41.0731403</v>
       </c>
       <c r="H70" t="n">
-        <v>37.3792617</v>
+        <v>27.4102013</v>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="n">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="B71" t="n">
-        <v>1956</v>
+        <v>1944</v>
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Giresun</t>
+          <t>Sakarya</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Adapazarı</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
@@ -2837,24 +2837,26 @@
       </c>
       <c r="F71" t="inlineStr">
         <is>
-          <t>Unknown, Giresun, Turkey</t>
+          <t>Adapazarı, Sakarya, Turkey</t>
         </is>
       </c>
       <c r="G71" t="n">
-        <v>40.6531617</v>
+        <v>40.7755188</v>
       </c>
       <c r="H71" t="n">
-        <v>38.5172032</v>
+        <v>30.4020898</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="n">
-        <v>1906</v>
-      </c>
-      <c r="B72" t="inlineStr"/>
+        <v>1904</v>
+      </c>
+      <c r="B72" t="n">
+        <v>1956</v>
+      </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Haifa</t>
+          <t>Alexandroupoli</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
@@ -2864,31 +2866,31 @@
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>Palestine</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F72" t="inlineStr">
         <is>
-          <t>Unknown, Haifa, Palestine</t>
+          <t>Unknown, Alexandroupoli, Greece</t>
         </is>
       </c>
       <c r="G72" t="n">
-        <v>32.8184911</v>
+        <v>40.845666</v>
       </c>
       <c r="H72" t="n">
-        <v>34.9988504</v>
+        <v>25.8778814</v>
       </c>
     </row>
     <row r="73">
       <c r="A73" t="n">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="B73" t="n">
-        <v>1958</v>
+        <v>1922</v>
       </c>
       <c r="C73" t="inlineStr">
         <is>
-          <t>Kütahya</t>
+          <t>Drama</t>
         </is>
       </c>
       <c r="D73" t="inlineStr">
@@ -2898,31 +2900,31 @@
       </c>
       <c r="E73" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F73" t="inlineStr">
         <is>
-          <t>Unknown, Kütahya, Turkey</t>
+          <t>Unknown, Drama, Greece</t>
         </is>
       </c>
       <c r="G73" t="n">
-        <v>39.2522508</v>
+        <v>41.1499443</v>
       </c>
       <c r="H73" t="n">
-        <v>29.4937732</v>
+        <v>24.1468286</v>
       </c>
     </row>
     <row r="74">
       <c r="A74" t="n">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="B74" t="n">
         <v>1956</v>
       </c>
       <c r="C74" t="inlineStr">
         <is>
-          <t>Latakia</t>
+          <t>Giresun</t>
         </is>
       </c>
       <c r="D74" t="inlineStr">
@@ -2932,31 +2934,29 @@
       </c>
       <c r="E74" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F74" t="inlineStr">
         <is>
-          <t>Unknown, Latakia, Syria</t>
+          <t>Unknown, Giresun, Turkey</t>
         </is>
       </c>
       <c r="G74" t="n">
-        <v>35.5200185</v>
+        <v>40.6531617</v>
       </c>
       <c r="H74" t="n">
-        <v>35.7781044</v>
+        <v>38.5172032</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" t="n">
-        <v>1906</v>
-      </c>
-      <c r="B75" t="n">
-        <v>1913</v>
-      </c>
+        <v>1904</v>
+      </c>
+      <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Sakarya</t>
+          <t>Jerusalem</t>
         </is>
       </c>
       <c r="D75" t="inlineStr">
@@ -2966,31 +2966,31 @@
       </c>
       <c r="E75" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Palestine</t>
         </is>
       </c>
       <c r="F75" t="inlineStr">
         <is>
-          <t>Unknown, Sakarya, Turkey</t>
+          <t>Unknown, Jerusalem, Palestine</t>
         </is>
       </c>
       <c r="G75" t="n">
-        <v>40.7731834</v>
+        <v>33.6132575</v>
       </c>
       <c r="H75" t="n">
-        <v>30.481606</v>
+        <v>-87.8553466</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="n">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="B76" t="n">
-        <v>1912</v>
+        <v>1932</v>
       </c>
       <c r="C76" t="inlineStr">
         <is>
-          <t>Tripoli</t>
+          <t>Kavala</t>
         </is>
       </c>
       <c r="D76" t="inlineStr">
@@ -3000,31 +3000,31 @@
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>Libya</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F76" t="inlineStr">
         <is>
-          <t>Unknown, Tripoli, Libya</t>
+          <t>Unknown, Kavala, Greece</t>
         </is>
       </c>
       <c r="G76" t="n">
-        <v>32.896672</v>
+        <v>40.9369224</v>
       </c>
       <c r="H76" t="n">
-        <v>13.1777923</v>
+        <v>24.4122766</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" t="n">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="B77" t="n">
-        <v>1913</v>
+        <v>1921</v>
       </c>
       <c r="C77" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Tripoli</t>
         </is>
       </c>
       <c r="D77" t="inlineStr">
@@ -3034,31 +3034,31 @@
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="F77" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, Egypt</t>
+          <t>Unknown, Tripoli, Lebanon</t>
         </is>
       </c>
       <c r="G77" t="n">
-        <v>26.2540493</v>
+        <v>34.4373616</v>
       </c>
       <c r="H77" t="n">
-        <v>29.2675469</v>
+        <v>35.8348551</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="n">
-        <v>1906</v>
+        <v>1904</v>
       </c>
       <c r="B78" t="n">
-        <v>1914</v>
+        <v>1933</v>
       </c>
       <c r="C78" t="inlineStr">
         <is>
-          <t>Xanthi</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D78" t="inlineStr">
@@ -3068,36 +3068,36 @@
       </c>
       <c r="E78" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F78" t="inlineStr">
         <is>
-          <t>Unknown, Xanthi, Greece</t>
+          <t>Unknown, Unknown, France</t>
         </is>
       </c>
       <c r="G78" t="n">
-        <v>41.13805</v>
+        <v>46.603354</v>
       </c>
       <c r="H78" t="n">
-        <v>24.8864089</v>
+        <v>1.8883335</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="n">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="B79" t="n">
-        <v>1944</v>
+        <v>1947</v>
       </c>
       <c r="C79" t="inlineStr">
         <is>
-          <t>Sakarya</t>
+          <t>Aydın</t>
         </is>
       </c>
       <c r="D79" t="inlineStr">
         <is>
-          <t>Adapazarı</t>
+          <t>Nazilli</t>
         </is>
       </c>
       <c r="E79" t="inlineStr">
@@ -3107,58 +3107,58 @@
       </c>
       <c r="F79" t="inlineStr">
         <is>
-          <t>Adapazarı, Sakarya, Turkey</t>
+          <t>Nazilli, Aydın, Turkey</t>
         </is>
       </c>
       <c r="G79" t="n">
-        <v>40.7755188</v>
+        <v>37.9097512</v>
       </c>
       <c r="H79" t="n">
-        <v>30.4020898</v>
+        <v>28.3242062</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="n">
-        <v>1907</v>
-      </c>
-      <c r="B80" t="inlineStr"/>
+        <v>1905</v>
+      </c>
+      <c r="B80" t="n">
+        <v>1950</v>
+      </c>
       <c r="C80" t="inlineStr">
         <is>
-          <t>Minya</t>
+          <t>Mersin</t>
         </is>
       </c>
       <c r="D80" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Tarsus</t>
         </is>
       </c>
       <c r="E80" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F80" t="inlineStr">
         <is>
-          <t>Unknown, Minya, Egypt</t>
+          <t>Tarsus, Mersin, Turkey</t>
         </is>
       </c>
       <c r="G80" t="n">
-        <v>28.2125404</v>
+        <v>36.9164834</v>
       </c>
       <c r="H80" t="n">
-        <v>30.9123741</v>
+        <v>34.895149</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="n">
-        <v>1907</v>
-      </c>
-      <c r="B81" t="n">
-        <v>1950</v>
-      </c>
+        <v>1905</v>
+      </c>
+      <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr">
         <is>
-          <t>Mosul</t>
+          <t>Jaffa</t>
         </is>
       </c>
       <c r="D81" t="inlineStr">
@@ -3168,31 +3168,31 @@
       </c>
       <c r="E81" t="inlineStr">
         <is>
-          <t>Iraq</t>
+          <t>Palestine</t>
         </is>
       </c>
       <c r="F81" t="inlineStr">
         <is>
-          <t>Unknown, Mosul, Iraq</t>
+          <t>Unknown, Jaffa, Palestine</t>
         </is>
       </c>
       <c r="G81" t="n">
-        <v>36.343694</v>
+        <v>32.0539873</v>
       </c>
       <c r="H81" t="n">
-        <v>43.0997156</v>
+        <v>34.75508</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="n">
-        <v>1907</v>
+        <v>1905</v>
       </c>
       <c r="B82" t="n">
-        <v>1928</v>
+        <v>1958</v>
       </c>
       <c r="C82" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Jerusalem</t>
         </is>
       </c>
       <c r="D82" t="inlineStr">
@@ -3202,99 +3202,99 @@
       </c>
       <c r="E82" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Israel</t>
         </is>
       </c>
       <c r="F82" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, Italy</t>
+          <t>Unknown, Jerusalem, Israel</t>
         </is>
       </c>
       <c r="G82" t="n">
-        <v>42.6384261</v>
+        <v>31.7788472</v>
       </c>
       <c r="H82" t="n">
-        <v>12.674297</v>
+        <v>35.2257856</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="n">
-        <v>1908</v>
+        <v>1905</v>
       </c>
       <c r="B83" t="n">
-        <v>1950</v>
+        <v>1919</v>
       </c>
       <c r="C83" t="inlineStr">
         <is>
-          <t>Mersin</t>
+          <t>Tripoli</t>
         </is>
       </c>
       <c r="D83" t="inlineStr">
         <is>
-          <t>Tarsus</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E83" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Libya</t>
         </is>
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Tarsus, Mersin, Turkey</t>
+          <t>Unknown, Tripoli, Libya</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>36.9164834</v>
+        <v>32.896672</v>
       </c>
       <c r="H83" t="n">
-        <v>34.895149</v>
+        <v>13.1777923</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="n">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="B84" t="n">
-        <v>1954</v>
+        <v>1907</v>
       </c>
       <c r="C84" t="inlineStr">
         <is>
-          <t>Amman</t>
+          <t>Mersin</t>
         </is>
       </c>
       <c r="D84" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Silifke</t>
         </is>
       </c>
       <c r="E84" t="inlineStr">
         <is>
-          <t>Jordan</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Unknown, Amman, Jordan</t>
+          <t>Silifke, Mersin, Turkey</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>31.9515694</v>
+        <v>36.3778166</v>
       </c>
       <c r="H84" t="n">
-        <v>35.9239625</v>
+        <v>33.9260372</v>
       </c>
     </row>
     <row r="85">
       <c r="A85" t="n">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="B85" t="n">
-        <v>1949</v>
+        <v>1955</v>
       </c>
       <c r="C85" t="inlineStr">
         <is>
-          <t>Arak</t>
+          <t>Erzurum</t>
         </is>
       </c>
       <c r="D85" t="inlineStr">
@@ -3304,31 +3304,31 @@
       </c>
       <c r="E85" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Unknown, Arak, Iran</t>
+          <t>Unknown, Erzurum, Turkey</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>34.0862719</v>
+        <v>39.90632</v>
       </c>
       <c r="H85" t="n">
-        <v>49.6893884</v>
+        <v>41.2727715</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" t="n">
-        <v>1908</v>
+        <v>1906</v>
       </c>
       <c r="B86" t="n">
-        <v>1921</v>
+        <v>1947</v>
       </c>
       <c r="C86" t="inlineStr">
         <is>
-          <t>Homs</t>
+          <t>Famagusta</t>
         </is>
       </c>
       <c r="D86" t="inlineStr">
@@ -3338,31 +3338,29 @@
       </c>
       <c r="E86" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Unknown, Homs, Syria</t>
+          <t>Unknown, Famagusta, Cyprus</t>
         </is>
       </c>
       <c r="G86" t="n">
-        <v>34.7333334</v>
+        <v>35.1205261</v>
       </c>
       <c r="H86" t="n">
-        <v>36.7166667</v>
+        <v>33.9387919</v>
       </c>
     </row>
     <row r="87">
       <c r="A87" t="n">
-        <v>1909</v>
-      </c>
-      <c r="B87" t="n">
-        <v>1921</v>
-      </c>
+        <v>1906</v>
+      </c>
+      <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
-          <t>Gümüşhane</t>
+          <t>Haifa</t>
         </is>
       </c>
       <c r="D87" t="inlineStr">
@@ -3372,31 +3370,31 @@
       </c>
       <c r="E87" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Palestine</t>
         </is>
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Unknown, Gümüşhane, Turkey</t>
+          <t>Unknown, Haifa, Palestine</t>
         </is>
       </c>
       <c r="G87" t="n">
-        <v>40.2533219</v>
+        <v>32.8184911</v>
       </c>
       <c r="H87" t="n">
-        <v>39.384968</v>
+        <v>34.9988504</v>
       </c>
     </row>
     <row r="88">
       <c r="A88" t="n">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="B88" t="n">
-        <v>1914</v>
+        <v>1956</v>
       </c>
       <c r="C88" t="inlineStr">
         <is>
-          <t>Komotini</t>
+          <t>Latakia</t>
         </is>
       </c>
       <c r="D88" t="inlineStr">
@@ -3406,31 +3404,31 @@
       </c>
       <c r="E88" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Syria</t>
         </is>
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Unknown, Komotini, Greece</t>
+          <t>Unknown, Latakia, Syria</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>41.1182</v>
+        <v>35.5200185</v>
       </c>
       <c r="H88" t="n">
-        <v>25.4035708</v>
+        <v>35.7781044</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="n">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="B89" t="n">
-        <v>1957</v>
+        <v>1913</v>
       </c>
       <c r="C89" t="inlineStr">
         <is>
-          <t>Tekirdağ</t>
+          <t>Sakarya</t>
         </is>
       </c>
       <c r="D89" t="inlineStr">
@@ -3445,22 +3443,22 @@
       </c>
       <c r="F89" t="inlineStr">
         <is>
-          <t>Unknown, Tekirdağ, Turkey</t>
+          <t>Unknown, Sakarya, Turkey</t>
         </is>
       </c>
       <c r="G89" t="n">
-        <v>41.0731403</v>
+        <v>40.7731834</v>
       </c>
       <c r="H89" t="n">
-        <v>27.4102013</v>
+        <v>30.481606</v>
       </c>
     </row>
     <row r="90">
       <c r="A90" t="n">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="B90" t="n">
-        <v>1934</v>
+        <v>1913</v>
       </c>
       <c r="C90" t="inlineStr">
         <is>
@@ -3474,31 +3472,31 @@
       </c>
       <c r="E90" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="F90" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, Syria</t>
+          <t>Unknown, Unknown, Egypt</t>
         </is>
       </c>
       <c r="G90" t="n">
-        <v>34.8147886</v>
+        <v>26.2540493</v>
       </c>
       <c r="H90" t="n">
-        <v>38.4231781</v>
+        <v>29.2675469</v>
       </c>
     </row>
     <row r="91">
       <c r="A91" t="n">
-        <v>1909</v>
+        <v>1906</v>
       </c>
       <c r="B91" t="n">
-        <v>1929</v>
+        <v>1914</v>
       </c>
       <c r="C91" t="inlineStr">
         <is>
-          <t>İznik</t>
+          <t>Xanthi</t>
         </is>
       </c>
       <c r="D91" t="inlineStr">
@@ -3508,36 +3506,36 @@
       </c>
       <c r="E91" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F91" t="inlineStr">
         <is>
-          <t>Unknown, İznik, Turkey</t>
+          <t>Unknown, Xanthi, Greece</t>
         </is>
       </c>
       <c r="G91" t="n">
-        <v>40.4303445</v>
+        <v>41.13805</v>
       </c>
       <c r="H91" t="n">
-        <v>29.7223732</v>
+        <v>24.8864089</v>
       </c>
     </row>
     <row r="92">
       <c r="A92" t="n">
-        <v>1910</v>
+        <v>1907</v>
       </c>
       <c r="B92" t="n">
-        <v>1926</v>
+        <v>1950</v>
       </c>
       <c r="C92" t="inlineStr">
         <is>
-          <t>Afyonkarahisar</t>
+          <t>Bitlis</t>
         </is>
       </c>
       <c r="D92" t="inlineStr">
         <is>
-          <t>Bolvadin</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E92" t="inlineStr">
@@ -3547,58 +3545,58 @@
       </c>
       <c r="F92" t="inlineStr">
         <is>
-          <t>Bolvadin, Afyonkarahisar, Turkey</t>
+          <t>Unknown, Bitlis, Turkey</t>
         </is>
       </c>
       <c r="G92" t="n">
-        <v>38.7115866</v>
+        <v>38.4950867</v>
       </c>
       <c r="H92" t="n">
-        <v>31.0454865</v>
+        <v>42.1678372</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="n">
-        <v>1910</v>
+        <v>1907</v>
       </c>
       <c r="B93" t="inlineStr"/>
       <c r="C93" t="inlineStr">
         <is>
-          <t>Sakarya</t>
+          <t>Minya</t>
         </is>
       </c>
       <c r="D93" t="inlineStr">
         <is>
-          <t>Geyve</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E93" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="F93" t="inlineStr">
         <is>
-          <t>Geyve, Sakarya, Turkey</t>
+          <t>Unknown, Minya, Egypt</t>
         </is>
       </c>
       <c r="G93" t="n">
-        <v>40.5090547</v>
+        <v>28.2125404</v>
       </c>
       <c r="H93" t="n">
-        <v>30.2902514</v>
+        <v>30.9123741</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" t="n">
-        <v>1910</v>
+        <v>1907</v>
       </c>
       <c r="B94" t="n">
-        <v>1921</v>
+        <v>1928</v>
       </c>
       <c r="C94" t="inlineStr">
         <is>
-          <t>Drama</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D94" t="inlineStr">
@@ -3608,31 +3606,31 @@
       </c>
       <c r="E94" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Unknown, Drama, Greece</t>
+          <t>Unknown, Unknown, Italy</t>
         </is>
       </c>
       <c r="G94" t="n">
-        <v>41.1499443</v>
+        <v>42.6384261</v>
       </c>
       <c r="H94" t="n">
-        <v>24.1468286</v>
+        <v>12.674297</v>
       </c>
     </row>
     <row r="95">
       <c r="A95" t="n">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="B95" t="n">
-        <v>1933</v>
+        <v>1954</v>
       </c>
       <c r="C95" t="inlineStr">
         <is>
-          <t>Elazığ</t>
+          <t>Amman</t>
         </is>
       </c>
       <c r="D95" t="inlineStr">
@@ -3642,31 +3640,31 @@
       </c>
       <c r="E95" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Jordan</t>
         </is>
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>Unknown, Elazığ, Turkey</t>
+          <t>Unknown, Amman, Jordan</t>
         </is>
       </c>
       <c r="G95" t="n">
-        <v>38.5824771</v>
+        <v>31.9515694</v>
       </c>
       <c r="H95" t="n">
-        <v>39.396179</v>
+        <v>35.9239625</v>
       </c>
     </row>
     <row r="96">
       <c r="A96" t="n">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="B96" t="n">
-        <v>1921</v>
+        <v>1949</v>
       </c>
       <c r="C96" t="inlineStr">
         <is>
-          <t>Ioannina</t>
+          <t>Arak</t>
         </is>
       </c>
       <c r="D96" t="inlineStr">
@@ -3676,31 +3674,31 @@
       </c>
       <c r="E96" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>Unknown, Ioannina, Greece</t>
+          <t>Unknown, Arak, Iran</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>39.6639818</v>
+        <v>34.0862719</v>
       </c>
       <c r="H96" t="n">
-        <v>20.8522784</v>
+        <v>49.6893884</v>
       </c>
     </row>
     <row r="97">
       <c r="A97" t="n">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="B97" t="n">
-        <v>1935</v>
+        <v>1957</v>
       </c>
       <c r="C97" t="inlineStr">
         <is>
-          <t>Kayseri</t>
+          <t>Hamadan</t>
         </is>
       </c>
       <c r="D97" t="inlineStr">
@@ -3710,29 +3708,31 @@
       </c>
       <c r="E97" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="F97" t="inlineStr">
         <is>
-          <t>Unknown, Kayseri, Turkey</t>
+          <t>Unknown, Hamadan, Iran</t>
         </is>
       </c>
       <c r="G97" t="n">
-        <v>38.7219011</v>
+        <v>34.9726302</v>
       </c>
       <c r="H97" t="n">
-        <v>35.4873214</v>
+        <v>48.6563818</v>
       </c>
     </row>
     <row r="98">
       <c r="A98" t="n">
-        <v>1910</v>
-      </c>
-      <c r="B98" t="inlineStr"/>
+        <v>1908</v>
+      </c>
+      <c r="B98" t="n">
+        <v>1921</v>
+      </c>
       <c r="C98" t="inlineStr">
         <is>
-          <t>Mansura</t>
+          <t>Homs</t>
         </is>
       </c>
       <c r="D98" t="inlineStr">
@@ -3742,31 +3742,31 @@
       </c>
       <c r="E98" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Syria</t>
         </is>
       </c>
       <c r="F98" t="inlineStr">
         <is>
-          <t>Unknown, Mansura, Egypt</t>
+          <t>Unknown, Homs, Syria</t>
         </is>
       </c>
       <c r="G98" t="n">
-        <v>31.037566</v>
+        <v>34.7333334</v>
       </c>
       <c r="H98" t="n">
-        <v>31.38649</v>
+        <v>36.7166667</v>
       </c>
     </row>
     <row r="99">
       <c r="A99" t="n">
-        <v>1910</v>
+        <v>1908</v>
       </c>
       <c r="B99" t="n">
-        <v>1957</v>
+        <v>1949</v>
       </c>
       <c r="C99" t="inlineStr">
         <is>
-          <t>Ordu</t>
+          <t>Kermanshah</t>
         </is>
       </c>
       <c r="D99" t="inlineStr">
@@ -3776,31 +3776,31 @@
       </c>
       <c r="E99" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Iran</t>
         </is>
       </c>
       <c r="F99" t="inlineStr">
         <is>
-          <t>Unknown, Ordu, Turkey</t>
+          <t>Unknown, Kermanshah, Iran</t>
         </is>
       </c>
       <c r="G99" t="n">
-        <v>40.8292569</v>
+        <v>34.486732</v>
       </c>
       <c r="H99" t="n">
-        <v>37.4082764</v>
+        <v>46.808727</v>
       </c>
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B100" t="n">
         <v>1921</v>
       </c>
       <c r="C100" t="inlineStr">
         <is>
-          <t>Serres</t>
+          <t>Gümüşhane</t>
         </is>
       </c>
       <c r="D100" t="inlineStr">
@@ -3810,29 +3810,31 @@
       </c>
       <c r="E100" t="inlineStr">
         <is>
-          <t>Greece</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F100" t="inlineStr">
         <is>
-          <t>Unknown, Serres, Greece</t>
+          <t>Unknown, Gümüşhane, Turkey</t>
         </is>
       </c>
       <c r="G100" t="n">
-        <v>41.0910711</v>
+        <v>40.2533219</v>
       </c>
       <c r="H100" t="n">
-        <v>23.5498031</v>
+        <v>39.384968</v>
       </c>
     </row>
     <row r="101">
       <c r="A101" t="n">
-        <v>1910</v>
-      </c>
-      <c r="B101" t="inlineStr"/>
+        <v>1909</v>
+      </c>
+      <c r="B101" t="n">
+        <v>1914</v>
+      </c>
       <c r="C101" t="inlineStr">
         <is>
-          <t>Soufli</t>
+          <t>Komotini</t>
         </is>
       </c>
       <c r="D101" t="inlineStr">
@@ -3847,65 +3849,65 @@
       </c>
       <c r="F101" t="inlineStr">
         <is>
-          <t>Unknown, Soufli, Greece</t>
+          <t>Unknown, Komotini, Greece</t>
         </is>
       </c>
       <c r="G101" t="n">
-        <v>41.1941684</v>
+        <v>41.1182</v>
       </c>
       <c r="H101" t="n">
-        <v>26.302313</v>
+        <v>25.4035708</v>
       </c>
     </row>
     <row r="102">
       <c r="A102" t="n">
-        <v>1910</v>
+        <v>1909</v>
       </c>
       <c r="B102" t="n">
-        <v>1957</v>
+        <v>1934</v>
       </c>
       <c r="C102" t="inlineStr">
         <is>
-          <t>Kastamonu</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D102" t="inlineStr">
         <is>
-          <t>İnebolu</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E102" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Syria</t>
         </is>
       </c>
       <c r="F102" t="inlineStr">
         <is>
-          <t>İnebolu, Kastamonu, Turkey</t>
+          <t>Unknown, Unknown, Syria</t>
         </is>
       </c>
       <c r="G102" t="n">
-        <v>41.9785763</v>
+        <v>34.8147886</v>
       </c>
       <c r="H102" t="n">
-        <v>33.7599031</v>
+        <v>38.4231781</v>
       </c>
     </row>
     <row r="103">
       <c r="A103" t="n">
-        <v>1911</v>
+        <v>1909</v>
       </c>
       <c r="B103" t="n">
-        <v>1948</v>
+        <v>1929</v>
       </c>
       <c r="C103" t="inlineStr">
         <is>
-          <t>Adana</t>
+          <t>İznik</t>
         </is>
       </c>
       <c r="D103" t="inlineStr">
         <is>
-          <t>Ceyhan</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E103" t="inlineStr">
@@ -3915,29 +3917,29 @@
       </c>
       <c r="F103" t="inlineStr">
         <is>
-          <t>Ceyhan, Adana, Turkey</t>
+          <t>Unknown, İznik, Turkey</t>
         </is>
       </c>
       <c r="G103" t="n">
-        <v>37.0288825</v>
+        <v>40.4303445</v>
       </c>
       <c r="H103" t="n">
-        <v>35.8124428</v>
+        <v>29.7223732</v>
       </c>
     </row>
     <row r="104">
       <c r="A104" t="n">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B104" t="inlineStr"/>
       <c r="C104" t="inlineStr">
         <is>
-          <t>Elazığ</t>
+          <t>Sakarya</t>
         </is>
       </c>
       <c r="D104" t="inlineStr">
         <is>
-          <t>Harput</t>
+          <t>Geyve</t>
         </is>
       </c>
       <c r="E104" t="inlineStr">
@@ -3947,26 +3949,26 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Harput, Elazığ, Turkey</t>
+          <t>Geyve, Sakarya, Turkey</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>38.7046229</v>
+        <v>40.5090547</v>
       </c>
       <c r="H104" t="n">
-        <v>39.2521174</v>
+        <v>30.2902514</v>
       </c>
     </row>
     <row r="105">
       <c r="A105" t="n">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B105" t="n">
-        <v>1921</v>
+        <v>1957</v>
       </c>
       <c r="C105" t="inlineStr">
         <is>
-          <t>Al Hudaydah</t>
+          <t>Bolu</t>
         </is>
       </c>
       <c r="D105" t="inlineStr">
@@ -3976,31 +3978,31 @@
       </c>
       <c r="E105" t="inlineStr">
         <is>
-          <t>Yemen</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Unknown, Al Hudaydah, Yemen</t>
+          <t>Unknown, Bolu, Turkey</t>
         </is>
       </c>
       <c r="G105" t="n">
-        <v>15.1159326</v>
+        <v>40.6212099</v>
       </c>
       <c r="H105" t="n">
-        <v>42.844785</v>
+        <v>31.6460259</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" t="n">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B106" t="n">
-        <v>1912</v>
+        <v>1933</v>
       </c>
       <c r="C106" t="inlineStr">
         <is>
-          <t>Benghazi</t>
+          <t>Elazığ</t>
         </is>
       </c>
       <c r="D106" t="inlineStr">
@@ -4010,31 +4012,31 @@
       </c>
       <c r="E106" t="inlineStr">
         <is>
-          <t>Libya</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F106" t="inlineStr">
         <is>
-          <t>Unknown, Benghazi, Libya</t>
+          <t>Unknown, Elazığ, Turkey</t>
         </is>
       </c>
       <c r="G106" t="n">
-        <v>32.1200168</v>
+        <v>38.5824771</v>
       </c>
       <c r="H106" t="n">
-        <v>20.0812174</v>
+        <v>39.396179</v>
       </c>
     </row>
     <row r="107">
       <c r="A107" t="n">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B107" t="n">
         <v>1950</v>
       </c>
       <c r="C107" t="inlineStr">
         <is>
-          <t>Bitlis</t>
+          <t>Ioannina</t>
         </is>
       </c>
       <c r="D107" t="inlineStr">
@@ -4044,31 +4046,31 @@
       </c>
       <c r="E107" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Unknown, Bitlis, Turkey</t>
+          <t>Unknown, Ioannina, Greece</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>38.4950867</v>
+        <v>39.6639818</v>
       </c>
       <c r="H107" t="n">
-        <v>42.1678372</v>
+        <v>20.8522784</v>
       </c>
     </row>
     <row r="108">
       <c r="A108" t="n">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B108" t="n">
         <v>1935</v>
       </c>
       <c r="C108" t="inlineStr">
         <is>
-          <t>Diyarbakır</t>
+          <t>Kayseri</t>
         </is>
       </c>
       <c r="D108" t="inlineStr">
@@ -4083,24 +4085,24 @@
       </c>
       <c r="F108" t="inlineStr">
         <is>
-          <t>Unknown, Diyarbakır, Turkey</t>
+          <t>Unknown, Kayseri, Turkey</t>
         </is>
       </c>
       <c r="G108" t="n">
-        <v>37.9162222</v>
+        <v>38.7219011</v>
       </c>
       <c r="H108" t="n">
-        <v>40.2363542</v>
+        <v>35.4873214</v>
       </c>
     </row>
     <row r="109">
       <c r="A109" t="n">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B109" t="inlineStr"/>
       <c r="C109" t="inlineStr">
         <is>
-          <t>Manchester</t>
+          <t>Mansura</t>
         </is>
       </c>
       <c r="D109" t="inlineStr">
@@ -4110,27 +4112,27 @@
       </c>
       <c r="E109" t="inlineStr">
         <is>
-          <t>United Kingdom</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="F109" t="inlineStr">
         <is>
-          <t>Unknown, Manchester, United Kingdom</t>
+          <t>Unknown, Mansura, Egypt</t>
         </is>
       </c>
       <c r="G109" t="n">
-        <v>53.4794892</v>
+        <v>31.037566</v>
       </c>
       <c r="H109" t="n">
-        <v>-2.2451148</v>
+        <v>31.38649</v>
       </c>
     </row>
     <row r="110">
       <c r="A110" t="n">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B110" t="n">
-        <v>1921</v>
+        <v>1933</v>
       </c>
       <c r="C110" t="inlineStr">
         <is>
@@ -4161,14 +4163,14 @@
     </row>
     <row r="111">
       <c r="A111" t="n">
-        <v>1911</v>
+        <v>1910</v>
       </c>
       <c r="B111" t="n">
-        <v>1914</v>
+        <v>1921</v>
       </c>
       <c r="C111" t="inlineStr">
         <is>
-          <t>Shkodra</t>
+          <t>Serres</t>
         </is>
       </c>
       <c r="D111" t="inlineStr">
@@ -4178,31 +4180,29 @@
       </c>
       <c r="E111" t="inlineStr">
         <is>
-          <t>Albania</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F111" t="inlineStr">
         <is>
-          <t>Unknown, Shkodra, Albania</t>
+          <t>Unknown, Serres, Greece</t>
         </is>
       </c>
       <c r="G111" t="n">
-        <v>42.0681371</v>
+        <v>41.0910711</v>
       </c>
       <c r="H111" t="n">
-        <v>19.5121437</v>
+        <v>23.5498031</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" t="n">
-        <v>1911</v>
-      </c>
-      <c r="B112" t="n">
-        <v>1921</v>
-      </c>
+        <v>1910</v>
+      </c>
+      <c r="B112" t="inlineStr"/>
       <c r="C112" t="inlineStr">
         <is>
-          <t>Sidon</t>
+          <t>Soufli</t>
         </is>
       </c>
       <c r="D112" t="inlineStr">
@@ -4212,19 +4212,19 @@
       </c>
       <c r="E112" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Greece</t>
         </is>
       </c>
       <c r="F112" t="inlineStr">
         <is>
-          <t>Unknown, Sidon, Lebanon</t>
+          <t>Unknown, Soufli, Greece</t>
         </is>
       </c>
       <c r="G112" t="n">
-        <v>33.5618345</v>
+        <v>41.1941684</v>
       </c>
       <c r="H112" t="n">
-        <v>35.3780338</v>
+        <v>26.302313</v>
       </c>
     </row>
     <row r="113">
@@ -4232,16 +4232,16 @@
         <v>1911</v>
       </c>
       <c r="B113" t="n">
-        <v>1920</v>
+        <v>1948</v>
       </c>
       <c r="C113" t="inlineStr">
         <is>
-          <t>Van</t>
+          <t>Adana</t>
         </is>
       </c>
       <c r="D113" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Ceyhan</t>
         </is>
       </c>
       <c r="E113" t="inlineStr">
@@ -4251,31 +4251,29 @@
       </c>
       <c r="F113" t="inlineStr">
         <is>
-          <t>Unknown, Van, Turkey</t>
+          <t>Ceyhan, Adana, Turkey</t>
         </is>
       </c>
       <c r="G113" t="n">
-        <v>38.3249599</v>
+        <v>37.0288825</v>
       </c>
       <c r="H113" t="n">
-        <v>43.6589825</v>
+        <v>35.8124428</v>
       </c>
     </row>
     <row r="114">
       <c r="A114" t="n">
-        <v>1912</v>
-      </c>
-      <c r="B114" t="n">
-        <v>1947</v>
-      </c>
+        <v>1911</v>
+      </c>
+      <c r="B114" t="inlineStr"/>
       <c r="C114" t="inlineStr">
         <is>
-          <t>Afyonkarahisar</t>
+          <t>Elazığ</t>
         </is>
       </c>
       <c r="D114" t="inlineStr">
         <is>
-          <t>Sandıklı</t>
+          <t>Harput</t>
         </is>
       </c>
       <c r="E114" t="inlineStr">
@@ -4285,58 +4283,60 @@
       </c>
       <c r="F114" t="inlineStr">
         <is>
-          <t>Sandıklı, Afyonkarahisar, Turkey</t>
+          <t>Harput, Elazığ, Turkey</t>
         </is>
       </c>
       <c r="G114" t="n">
-        <v>38.4647643</v>
+        <v>38.7046229</v>
       </c>
       <c r="H114" t="n">
-        <v>30.272542</v>
+        <v>39.2521174</v>
       </c>
     </row>
     <row r="115">
       <c r="A115" t="n">
-        <v>1912</v>
-      </c>
-      <c r="B115" t="inlineStr"/>
+        <v>1911</v>
+      </c>
+      <c r="B115" t="n">
+        <v>1921</v>
+      </c>
       <c r="C115" t="inlineStr">
         <is>
-          <t>Aydın</t>
+          <t>Al Hudaydah</t>
         </is>
       </c>
       <c r="D115" t="inlineStr">
         <is>
-          <t>Söke</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E115" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Yemen</t>
         </is>
       </c>
       <c r="F115" t="inlineStr">
         <is>
-          <t>Söke, Aydın, Turkey</t>
+          <t>Unknown, Al Hudaydah, Yemen</t>
         </is>
       </c>
       <c r="G115" t="n">
-        <v>37.7519762</v>
+        <v>15.1159326</v>
       </c>
       <c r="H115" t="n">
-        <v>27.4056294</v>
+        <v>42.844785</v>
       </c>
     </row>
     <row r="116">
       <c r="A116" t="n">
+        <v>1911</v>
+      </c>
+      <c r="B116" t="n">
         <v>1912</v>
       </c>
-      <c r="B116" t="n">
-        <v>1957</v>
-      </c>
       <c r="C116" t="inlineStr">
         <is>
-          <t>Bolu</t>
+          <t>Benghazi</t>
         </is>
       </c>
       <c r="D116" t="inlineStr">
@@ -4346,31 +4346,29 @@
       </c>
       <c r="E116" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Libya</t>
         </is>
       </c>
       <c r="F116" t="inlineStr">
         <is>
-          <t>Unknown, Bolu, Turkey</t>
+          <t>Unknown, Benghazi, Libya</t>
         </is>
       </c>
       <c r="G116" t="n">
-        <v>40.6212099</v>
+        <v>32.1200168</v>
       </c>
       <c r="H116" t="n">
-        <v>31.6460259</v>
+        <v>20.0812174</v>
       </c>
     </row>
     <row r="117">
       <c r="A117" t="n">
-        <v>1912</v>
-      </c>
-      <c r="B117" t="n">
-        <v>1916</v>
-      </c>
+        <v>1911</v>
+      </c>
+      <c r="B117" t="inlineStr"/>
       <c r="C117" t="inlineStr">
         <is>
-          <t>Jeddah</t>
+          <t>Manchester</t>
         </is>
       </c>
       <c r="D117" t="inlineStr">
@@ -4380,31 +4378,31 @@
       </c>
       <c r="E117" t="inlineStr">
         <is>
-          <t>Saudi Arabia</t>
+          <t>United Kingdom</t>
         </is>
       </c>
       <c r="F117" t="inlineStr">
         <is>
-          <t>Unknown, Jeddah, Saudi Arabia</t>
+          <t>Unknown, Manchester, United Kingdom</t>
         </is>
       </c>
       <c r="G117" t="n">
-        <v>21.5504432</v>
+        <v>53.4794892</v>
       </c>
       <c r="H117" t="n">
-        <v>39.1742363</v>
+        <v>-2.2451148</v>
       </c>
     </row>
     <row r="118">
       <c r="A118" t="n">
-        <v>1912</v>
+        <v>1911</v>
       </c>
       <c r="B118" t="n">
-        <v>1934</v>
+        <v>1914</v>
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Şanlıurfa</t>
+          <t>Shkodra</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
@@ -4414,65 +4412,65 @@
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Albania</t>
         </is>
       </c>
       <c r="F118" t="inlineStr">
         <is>
-          <t>Unknown, Şanlıurfa, Turkey</t>
+          <t>Unknown, Shkodra, Albania</t>
         </is>
       </c>
       <c r="G118" t="n">
-        <v>37.2595198</v>
+        <v>42.0681371</v>
       </c>
       <c r="H118" t="n">
-        <v>39.0408174</v>
+        <v>19.5121437</v>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="n">
-        <v>1913</v>
+        <v>1911</v>
       </c>
       <c r="B119" t="n">
         <v>1921</v>
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Hatay</t>
+          <t>Sidon</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>İskenderun</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="F119" t="inlineStr">
         <is>
-          <t>İskenderun, Hatay, Turkey</t>
+          <t>Unknown, Sidon, Lebanon</t>
         </is>
       </c>
       <c r="G119" t="n">
-        <v>36.5902266</v>
+        <v>33.5618345</v>
       </c>
       <c r="H119" t="n">
-        <v>36.1710354</v>
+        <v>35.3780338</v>
       </c>
     </row>
     <row r="120">
       <c r="A120" t="n">
-        <v>1914</v>
+        <v>1911</v>
       </c>
       <c r="B120" t="n">
-        <v>1958</v>
+        <v>1920</v>
       </c>
       <c r="C120" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Van</t>
         </is>
       </c>
       <c r="D120" t="inlineStr">
@@ -4482,36 +4480,36 @@
       </c>
       <c r="E120" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F120" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, Cyprus</t>
+          <t>Unknown, Van, Turkey</t>
         </is>
       </c>
       <c r="G120" t="n">
-        <v>34.9174159</v>
+        <v>38.3249599</v>
       </c>
       <c r="H120" t="n">
-        <v>32.8899027</v>
+        <v>43.6589825</v>
       </c>
     </row>
     <row r="121">
       <c r="A121" t="n">
-        <v>1914</v>
+        <v>1912</v>
       </c>
       <c r="B121" t="n">
-        <v>1950</v>
+        <v>1947</v>
       </c>
       <c r="C121" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Afyonkarahisar</t>
         </is>
       </c>
       <c r="D121" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Sandıklı</t>
         </is>
       </c>
       <c r="E121" t="inlineStr">
@@ -4521,63 +4519,63 @@
       </c>
       <c r="F121" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, Turkey</t>
+          <t>Sandıklı, Afyonkarahisar, Turkey</t>
         </is>
       </c>
       <c r="G121" t="n">
-        <v>39.294076</v>
+        <v>38.4647643</v>
       </c>
       <c r="H121" t="n">
-        <v>35.2316631</v>
+        <v>30.272542</v>
       </c>
     </row>
     <row r="122">
       <c r="A122" t="n">
-        <v>1914</v>
-      </c>
-      <c r="B122" t="n">
-        <v>1921</v>
-      </c>
+        <v>1912</v>
+      </c>
+      <c r="B122" t="inlineStr"/>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Zahle</t>
+          <t>Aydın</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Söke</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F122" t="inlineStr">
         <is>
-          <t>Unknown, Zahle, Lebanon</t>
+          <t>Söke, Aydın, Turkey</t>
         </is>
       </c>
       <c r="G122" t="n">
-        <v>33.8477069</v>
+        <v>37.7519762</v>
       </c>
       <c r="H122" t="n">
-        <v>35.9024955</v>
+        <v>27.4056294</v>
       </c>
     </row>
     <row r="123">
       <c r="A123" t="n">
-        <v>1914</v>
-      </c>
-      <c r="B123" t="inlineStr"/>
+        <v>1913</v>
+      </c>
+      <c r="B123" t="n">
+        <v>1921</v>
+      </c>
       <c r="C123" t="inlineStr">
         <is>
-          <t>Çanakkale</t>
+          <t>Hatay</t>
         </is>
       </c>
       <c r="D123" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>İskenderun</t>
         </is>
       </c>
       <c r="E123" t="inlineStr">
@@ -4587,24 +4585,26 @@
       </c>
       <c r="F123" t="inlineStr">
         <is>
-          <t>Unknown, Çanakkale, Turkey</t>
+          <t>İskenderun, Hatay, Turkey</t>
         </is>
       </c>
       <c r="G123" t="n">
-        <v>40.0549886</v>
+        <v>36.5902266</v>
       </c>
       <c r="H123" t="n">
-        <v>26.9278292</v>
+        <v>36.1710354</v>
       </c>
     </row>
     <row r="124">
       <c r="A124" t="n">
-        <v>1915</v>
-      </c>
-      <c r="B124" t="inlineStr"/>
+        <v>1914</v>
+      </c>
+      <c r="B124" t="n">
+        <v>1958</v>
+      </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Marseille</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
@@ -4614,31 +4614,31 @@
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>France</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="F124" t="inlineStr">
         <is>
-          <t>Unknown, Marseille, France</t>
+          <t>Unknown, Unknown, Cyprus</t>
         </is>
       </c>
       <c r="G124" t="n">
-        <v>43.2961743</v>
+        <v>34.9174159</v>
       </c>
       <c r="H124" t="n">
-        <v>5.3699525</v>
+        <v>32.8899027</v>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="n">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="B125" t="n">
-        <v>1951</v>
+        <v>1950</v>
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Mansoura</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
@@ -4648,31 +4648,31 @@
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>Egypt</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F125" t="inlineStr">
         <is>
-          <t>Unknown, Mansoura, Egypt</t>
+          <t>Unknown, Unknown, Turkey</t>
         </is>
       </c>
       <c r="G125" t="n">
-        <v>31.0407772</v>
+        <v>39.294076</v>
       </c>
       <c r="H125" t="n">
-        <v>31.3581295</v>
+        <v>35.2316631</v>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="n">
-        <v>1916</v>
+        <v>1914</v>
       </c>
       <c r="B126" t="n">
-        <v>1932</v>
+        <v>1921</v>
       </c>
       <c r="C126" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Zahle</t>
         </is>
       </c>
       <c r="D126" t="inlineStr">
@@ -4682,31 +4682,29 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>Iraq</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="F126" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, Iraq</t>
+          <t>Unknown, Zahle, Lebanon</t>
         </is>
       </c>
       <c r="G126" t="n">
-        <v>33.0955793</v>
+        <v>33.8477069</v>
       </c>
       <c r="H126" t="n">
-        <v>44.1749775</v>
+        <v>35.9024955</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" t="n">
-        <v>1917</v>
-      </c>
-      <c r="B127" t="n">
-        <v>1957</v>
-      </c>
+        <v>1914</v>
+      </c>
+      <c r="B127" t="inlineStr"/>
       <c r="C127" t="inlineStr">
         <is>
-          <t>Naples</t>
+          <t>Çanakkale</t>
         </is>
       </c>
       <c r="D127" t="inlineStr">
@@ -4716,65 +4714,63 @@
       </c>
       <c r="E127" t="inlineStr">
         <is>
-          <t>Italy</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F127" t="inlineStr">
         <is>
-          <t>Unknown, Naples, Italy</t>
+          <t>Unknown, Çanakkale, Turkey</t>
         </is>
       </c>
       <c r="G127" t="n">
-        <v>40.8358846</v>
+        <v>40.0549886</v>
       </c>
       <c r="H127" t="n">
-        <v>14.2487679</v>
+        <v>26.9278292</v>
       </c>
     </row>
     <row r="128">
       <c r="A128" t="n">
-        <v>1919</v>
-      </c>
-      <c r="B128" t="n">
-        <v>1934</v>
-      </c>
+        <v>1915</v>
+      </c>
+      <c r="B128" t="inlineStr"/>
       <c r="C128" t="inlineStr">
         <is>
-          <t>Muğla</t>
+          <t>Marseille</t>
         </is>
       </c>
       <c r="D128" t="inlineStr">
         <is>
-          <t>Milas</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>Turkey</t>
+          <t>France</t>
         </is>
       </c>
       <c r="F128" t="inlineStr">
         <is>
-          <t>Milas, Muğla, Turkey</t>
+          <t>Unknown, Marseille, France</t>
         </is>
       </c>
       <c r="G128" t="n">
-        <v>37.3162709</v>
+        <v>43.2961743</v>
       </c>
       <c r="H128" t="n">
-        <v>27.7799762</v>
+        <v>5.3699525</v>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="n">
-        <v>1919</v>
+        <v>1916</v>
       </c>
       <c r="B129" t="n">
-        <v>1921</v>
+        <v>1951</v>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Hama</t>
+          <t>Mansoura</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
@@ -4784,27 +4780,27 @@
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>Syria</t>
+          <t>Egypt</t>
         </is>
       </c>
       <c r="F129" t="inlineStr">
         <is>
-          <t>Unknown, Hama, Syria</t>
+          <t>Unknown, Mansoura, Egypt</t>
         </is>
       </c>
       <c r="G129" t="n">
-        <v>35.1343368</v>
+        <v>31.0407772</v>
       </c>
       <c r="H129" t="n">
-        <v>36.7496276</v>
+        <v>31.3581295</v>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="n">
-        <v>1919</v>
+        <v>1916</v>
       </c>
       <c r="B130" t="n">
-        <v>1919</v>
+        <v>1932</v>
       </c>
       <c r="C130" t="inlineStr">
         <is>
@@ -4818,95 +4814,99 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>Lebanon</t>
+          <t>Iraq</t>
         </is>
       </c>
       <c r="F130" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, Lebanon</t>
+          <t>Unknown, Unknown, Iraq</t>
         </is>
       </c>
       <c r="G130" t="n">
-        <v>33.8750629</v>
+        <v>33.0955793</v>
       </c>
       <c r="H130" t="n">
-        <v>35.843409</v>
+        <v>44.1749775</v>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="n">
-        <v>1920</v>
-      </c>
-      <c r="B131" t="inlineStr"/>
+        <v>1917</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1957</v>
+      </c>
       <c r="C131" t="inlineStr">
         <is>
-          <t>Basra</t>
+          <t>Naples</t>
         </is>
       </c>
       <c r="D131" t="inlineStr">
         <is>
-          <t>Ashar</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>Iraq</t>
+          <t>Italy</t>
         </is>
       </c>
       <c r="F131" t="inlineStr">
         <is>
-          <t>Ashar, Basra, Iraq</t>
+          <t>Unknown, Naples, Italy</t>
         </is>
       </c>
       <c r="G131" t="n">
-        <v>30.5219014</v>
+        <v>40.8358846</v>
       </c>
       <c r="H131" t="n">
-        <v>47.8343864</v>
+        <v>14.2487679</v>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="n">
-        <v>1920</v>
+        <v>1919</v>
       </c>
       <c r="B132" t="n">
-        <v>1949</v>
+        <v>1934</v>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Kermanshah</t>
+          <t>Muğla</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Milas</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Turkey</t>
         </is>
       </c>
       <c r="F132" t="inlineStr">
         <is>
-          <t>Unknown, Kermanshah, Iran</t>
+          <t>Milas, Muğla, Turkey</t>
         </is>
       </c>
       <c r="G132" t="n">
-        <v>34.486732</v>
+        <v>37.3162709</v>
       </c>
       <c r="H132" t="n">
-        <v>46.808727</v>
+        <v>27.7799762</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="n">
-        <v>1920</v>
-      </c>
-      <c r="B133" t="inlineStr"/>
+        <v>1919</v>
+      </c>
+      <c r="B133" t="n">
+        <v>1919</v>
+      </c>
       <c r="C133" t="inlineStr">
         <is>
-          <t>Kirkuk</t>
+          <t>Unknown</t>
         </is>
       </c>
       <c r="D133" t="inlineStr">
@@ -4916,59 +4916,61 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>Iraq</t>
+          <t>Lebanon</t>
         </is>
       </c>
       <c r="F133" t="inlineStr">
         <is>
-          <t>Unknown, Kirkuk, Iraq</t>
+          <t>Unknown, Unknown, Lebanon</t>
         </is>
       </c>
       <c r="G133" t="n">
-        <v>35.4719308</v>
+        <v>33.8750629</v>
       </c>
       <c r="H133" t="n">
-        <v>44.3953896</v>
+        <v>35.843409</v>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="n">
         <v>1920</v>
       </c>
-      <c r="B134" t="n">
-        <v>1974</v>
-      </c>
+      <c r="B134" t="inlineStr"/>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Basra</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Ashar</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>Unknown</t>
+          <t>Iraq</t>
         </is>
       </c>
       <c r="F134" t="inlineStr">
         <is>
-          <t>Unknown, Unknown, Unknown</t>
-        </is>
-      </c>
-      <c r="G134" t="inlineStr"/>
-      <c r="H134" t="inlineStr"/>
+          <t>Ashar, Basra, Iraq</t>
+        </is>
+      </c>
+      <c r="G134" t="n">
+        <v>30.5219014</v>
+      </c>
+      <c r="H134" t="n">
+        <v>47.8343864</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135" t="n">
-        <v>1921</v>
+        <v>1920</v>
       </c>
       <c r="B135" t="inlineStr"/>
       <c r="C135" t="inlineStr">
         <is>
-          <t>Paphos</t>
+          <t>Kirkuk</t>
         </is>
       </c>
       <c r="D135" t="inlineStr">
@@ -4978,19 +4980,19 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>Cyprus</t>
+          <t>Iraq</t>
         </is>
       </c>
       <c r="F135" t="inlineStr">
         <is>
-          <t>Unknown, Paphos, Cyprus</t>
+          <t>Unknown, Kirkuk, Iraq</t>
         </is>
       </c>
       <c r="G135" t="n">
-        <v>34.7743988</v>
+        <v>35.4719308</v>
       </c>
       <c r="H135" t="n">
-        <v>32.4231586</v>
+        <v>44.3953896</v>
       </c>
     </row>
     <row r="136">
@@ -5000,7 +5002,7 @@
       <c r="B136" t="inlineStr"/>
       <c r="C136" t="inlineStr">
         <is>
-          <t>Troodos</t>
+          <t>Paphos</t>
         </is>
       </c>
       <c r="D136" t="inlineStr">
@@ -5015,26 +5017,24 @@
       </c>
       <c r="F136" t="inlineStr">
         <is>
-          <t>Unknown, Troodos, Cyprus</t>
+          <t>Unknown, Paphos, Cyprus</t>
         </is>
       </c>
       <c r="G136" t="n">
-        <v>34.9233165</v>
+        <v>34.7743988</v>
       </c>
       <c r="H136" t="n">
-        <v>32.8776077</v>
+        <v>32.4231586</v>
       </c>
     </row>
     <row r="137">
       <c r="A137" t="n">
         <v>1921</v>
       </c>
-      <c r="B137" t="n">
-        <v>1933</v>
-      </c>
+      <c r="B137" t="inlineStr"/>
       <c r="C137" t="inlineStr">
         <is>
-          <t>Tunis</t>
+          <t>Troodos</t>
         </is>
       </c>
       <c r="D137" t="inlineStr">
@@ -5044,29 +5044,31 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>Tunisia</t>
+          <t>Cyprus</t>
         </is>
       </c>
       <c r="F137" t="inlineStr">
         <is>
-          <t>Unknown, Tunis, Tunisia</t>
+          <t>Unknown, Troodos, Cyprus</t>
         </is>
       </c>
       <c r="G137" t="n">
-        <v>33.8439408</v>
+        <v>34.9233165</v>
       </c>
       <c r="H137" t="n">
-        <v>9.400138</v>
+        <v>32.8776077</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="n">
-        <v>1922</v>
-      </c>
-      <c r="B138" t="inlineStr"/>
+        <v>1921</v>
+      </c>
+      <c r="B138" t="n">
+        <v>1933</v>
+      </c>
       <c r="C138" t="inlineStr">
         <is>
-          <t>Bethlehem</t>
+          <t>Tunis</t>
         </is>
       </c>
       <c r="D138" t="inlineStr">
@@ -5076,31 +5078,29 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>Palestine</t>
+          <t>Tunisia</t>
         </is>
       </c>
       <c r="F138" t="inlineStr">
         <is>
-          <t>Unknown, Bethlehem, Palestine</t>
+          <t>Unknown, Tunis, Tunisia</t>
         </is>
       </c>
       <c r="G138" t="n">
-        <v>31.7059708</v>
+        <v>33.8439408</v>
       </c>
       <c r="H138" t="n">
-        <v>35.1877002</v>
+        <v>9.400138</v>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="n">
         <v>1922</v>
       </c>
-      <c r="B139" t="n">
-        <v>1957</v>
-      </c>
+      <c r="B139" t="inlineStr"/>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Hamadan</t>
+          <t>Bethlehem</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
@@ -5110,19 +5110,19 @@
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>Iran</t>
+          <t>Palestine</t>
         </is>
       </c>
       <c r="F139" t="inlineStr">
         <is>
-          <t>Unknown, Hamadan, Iran</t>
+          <t>Unknown, Bethlehem, Palestine</t>
         </is>
       </c>
       <c r="G139" t="n">
-        <v>34.9726302</v>
+        <v>31.7059708</v>
       </c>
       <c r="H139" t="n">
-        <v>48.6563818</v>
+        <v>35.1877002</v>
       </c>
     </row>
     <row r="140">

</xml_diff>